<commit_message>
schema tweaks and updating storybook
</commit_message>
<xml_diff>
--- a/payment_history.xlsx
+++ b/payment_history.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lydiacupery/Desktop/lydia/buying house docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lydiacupery/loan-calculator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACEA318E-EF9C-0E44-B83D-4AC821E341D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F074EB-3ED2-4840-892E-871B71307420}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="17920" windowHeight="21400" xr2:uid="{F3344CF8-01A7-4F48-A797-039A6BCEAE44}"/>
+    <workbookView xWindow="-25940" yWindow="-40" windowWidth="17920" windowHeight="21140" xr2:uid="{F3344CF8-01A7-4F48-A797-039A6BCEAE44}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="InterestRate">Sheet1!$E$4</definedName>
     <definedName name="LoanStartDate">Sheet1!$E$7</definedName>
+    <definedName name="PaymentsPerYear">Sheet1!$E$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -128,7 +130,44 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Table Amount" xfId="2" xr:uid="{B7D64A0B-C7BB-5446-8D89-BC0AC5C2E546}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -441,7 +480,7 @@
   <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -749,69 +788,116 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="1"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
+      <c r="A28" s="1">
+        <v>44145</v>
+      </c>
+      <c r="B28" s="3">
+        <v>1795.265347114811</v>
+      </c>
+      <c r="C28" s="3">
+        <v>240.29465288518907</v>
+      </c>
       <c r="D28" s="3"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="1"/>
+      <c r="A29" s="1">
+        <v>44175</v>
+      </c>
+      <c r="B29" s="3">
+        <v>1799.7535104825979</v>
+      </c>
+      <c r="C29" s="3">
+        <v>235.80648951740204</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="1"/>
+      <c r="A30" s="1">
+        <v>44206</v>
+      </c>
+      <c r="B30" s="3">
+        <v>2304.2528942588042</v>
+      </c>
+      <c r="C30" s="3">
+        <v>231.30710574119556</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B43" s="3"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
create a withMaxForDateForLoan dataloader - name could probably be improved...
</commit_message>
<xml_diff>
--- a/payment_history.xlsx
+++ b/payment_history.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lydiacupery/loan-calculator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F074EB-3ED2-4840-892E-871B71307420}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02BEE54-8F5A-094E-927A-855616F368D7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25940" yWindow="-40" windowWidth="17920" windowHeight="21140" xr2:uid="{F3344CF8-01A7-4F48-A797-039A6BCEAE44}"/>
   </bookViews>
@@ -480,7 +480,7 @@
   <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -822,9 +822,15 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="1"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
+      <c r="A31" s="1">
+        <v>44237</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1810.0135264944515</v>
+      </c>
+      <c r="C31" s="3">
+        <v>225.54647350554853</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>

</xml_diff>